<commit_message>
Add initial database handler
</commit_message>
<xml_diff>
--- a/PolarReport/TestData/2016/April/report_GaryCooper.xlsx
+++ b/PolarReport/TestData/2016/April/report_GaryCooper.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="9960"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="9960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Yleistiedot" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="44">
   <si>
     <t>Yritys</t>
   </si>
@@ -156,6 +156,21 @@
   <si>
     <t>gary.cooper@a-company.com</t>
   </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>Edell. kk kertymä</t>
+  </si>
+  <si>
+    <t>Muu poissaolo</t>
+  </si>
+  <si>
+    <t>Sairasloma</t>
+  </si>
+  <si>
+    <t>Loma</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +184,7 @@
     <numFmt numFmtId="168" formatCode="#,##0&quot; €&quot;"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Arial"/>
@@ -299,8 +314,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,8 +368,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="62">
+  <borders count="79">
     <border>
       <left/>
       <right/>
@@ -1083,13 +1114,238 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="261">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1476,6 +1732,197 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1518,231 +1965,185 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="21" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1751,7 +2152,63 @@
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
     <cellStyle name="Otsikko 1 1" xfId="2"/>
   </cellStyles>
-  <dxfs count="198">
+  <dxfs count="202">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <sz val="12"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="27"/>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <sz val="12"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="41"/>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <sz val="12"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="27"/>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <sz val="12"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="41"/>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4914,7 +5371,7 @@
   <sheetPr codeName="Taul1"/>
   <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showOutlineSymbols="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" showOutlineSymbols="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -5077,10 +5534,10 @@
   <sheetPr codeName="Taul2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AQ117"/>
+  <dimension ref="B1:AQ121"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" showOutlineSymbols="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:C45"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showOutlineSymbols="0" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5105,36 +5562,36 @@
   <sheetData>
     <row r="1" spans="2:43" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:43" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="215">
+      <c r="B2" s="170">
         <f>Yleistiedot!D4</f>
         <v>0</v>
       </c>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
       <c r="I2" s="25"/>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
-      <c r="M2" s="196">
+      <c r="M2" s="146">
         <f>H7</f>
         <v>42461</v>
       </c>
-      <c r="N2" s="196"/>
-      <c r="O2" s="196"/>
-      <c r="P2" s="196"/>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="196"/>
-      <c r="S2" s="196"/>
-      <c r="T2" s="196"/>
-      <c r="U2" s="196"/>
-      <c r="V2" s="196"/>
-      <c r="W2" s="196"/>
-      <c r="X2" s="196"/>
-      <c r="Y2" s="196"/>
+      <c r="N2" s="146"/>
+      <c r="O2" s="146"/>
+      <c r="P2" s="146"/>
+      <c r="Q2" s="146"/>
+      <c r="R2" s="146"/>
+      <c r="S2" s="146"/>
+      <c r="T2" s="146"/>
+      <c r="U2" s="146"/>
+      <c r="V2" s="146"/>
+      <c r="W2" s="146"/>
+      <c r="X2" s="146"/>
+      <c r="Y2" s="146"/>
       <c r="Z2" s="24"/>
       <c r="AA2" s="24"/>
       <c r="AB2" s="24"/>
@@ -5152,38 +5609,38 @@
       <c r="AN2" s="24"/>
       <c r="AO2" s="26">
         <f ca="1">TODAY()</f>
-        <v>42485</v>
+        <v>42488</v>
       </c>
       <c r="AP2" s="27"/>
     </row>
     <row r="3" spans="2:43" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="188" t="str">
+      <c r="B3" s="134" t="str">
         <f>Yleistiedot!D7</f>
         <v>Gary Cooper</v>
       </c>
-      <c r="C3" s="189"/>
-      <c r="D3" s="189"/>
-      <c r="E3" s="190"/>
-      <c r="F3" s="190"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
       <c r="L3" s="28"/>
-      <c r="M3" s="197"/>
-      <c r="N3" s="197"/>
-      <c r="O3" s="197"/>
-      <c r="P3" s="197"/>
-      <c r="Q3" s="197"/>
-      <c r="R3" s="197"/>
-      <c r="S3" s="197"/>
-      <c r="T3" s="197"/>
-      <c r="U3" s="197"/>
-      <c r="V3" s="197"/>
-      <c r="W3" s="197"/>
-      <c r="X3" s="197"/>
-      <c r="Y3" s="197"/>
+      <c r="M3" s="147"/>
+      <c r="N3" s="147"/>
+      <c r="O3" s="147"/>
+      <c r="P3" s="147"/>
+      <c r="Q3" s="147"/>
+      <c r="R3" s="147"/>
+      <c r="S3" s="147"/>
+      <c r="T3" s="147"/>
+      <c r="U3" s="147"/>
+      <c r="V3" s="147"/>
+      <c r="W3" s="147"/>
+      <c r="X3" s="147"/>
+      <c r="Y3" s="147"/>
       <c r="Z3" s="29"/>
       <c r="AA3" s="30"/>
       <c r="AB3" s="30"/>
@@ -5203,27 +5660,27 @@
       <c r="AP3" s="27"/>
     </row>
     <row r="4" spans="2:43" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="213" t="str">
+      <c r="B4" s="168" t="str">
         <f>Yleistiedot!D8</f>
         <v>gary.cooper@a-company.com</v>
       </c>
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
-      <c r="M4" s="197"/>
-      <c r="N4" s="197"/>
-      <c r="O4" s="197"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="197"/>
-      <c r="R4" s="197"/>
-      <c r="S4" s="197"/>
-      <c r="T4" s="197"/>
-      <c r="U4" s="197"/>
-      <c r="V4" s="197"/>
-      <c r="W4" s="197"/>
-      <c r="X4" s="197"/>
-      <c r="Y4" s="197"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="M4" s="147"/>
+      <c r="N4" s="147"/>
+      <c r="O4" s="147"/>
+      <c r="P4" s="147"/>
+      <c r="Q4" s="147"/>
+      <c r="R4" s="147"/>
+      <c r="S4" s="147"/>
+      <c r="T4" s="147"/>
+      <c r="U4" s="147"/>
+      <c r="V4" s="147"/>
+      <c r="W4" s="147"/>
+      <c r="X4" s="147"/>
+      <c r="Y4" s="147"/>
       <c r="Z4" s="29"/>
       <c r="AA4" s="32"/>
       <c r="AB4" s="32"/>
@@ -5235,11 +5692,11 @@
       <c r="AP4" s="27"/>
     </row>
     <row r="5" spans="2:43" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="191"/>
-      <c r="C5" s="192"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
+      <c r="B5" s="137"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
       <c r="G5" s="35"/>
       <c r="H5" s="126">
         <f>IF(H8="Su",1,IF(H8="La",1,0))</f>
@@ -5371,18 +5828,18 @@
       <c r="AP5" s="27"/>
     </row>
     <row r="6" spans="2:43" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="204" t="s">
+      <c r="B6" s="154" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="205"/>
-      <c r="D6" s="198" t="s">
+      <c r="C6" s="155"/>
+      <c r="D6" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="199"/>
-      <c r="F6" s="210" t="s">
+      <c r="E6" s="149"/>
+      <c r="F6" s="160" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="172"/>
+      <c r="G6" s="173"/>
       <c r="H6" s="38" t="s">
         <v>13</v>
       </c>
@@ -5424,12 +5881,12 @@
       <c r="AP6" s="27"/>
     </row>
     <row r="7" spans="2:43" ht="12.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="206"/>
-      <c r="C7" s="207"/>
-      <c r="D7" s="200"/>
-      <c r="E7" s="201"/>
-      <c r="F7" s="211"/>
-      <c r="G7" s="172"/>
+      <c r="B7" s="156"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="150"/>
+      <c r="E7" s="151"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="173"/>
       <c r="H7" s="45">
         <f>Yleistiedot!D5</f>
         <v>42461</v>
@@ -5567,12 +6024,12 @@
       <c r="AP7" s="27"/>
     </row>
     <row r="8" spans="2:43" ht="12.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="206"/>
-      <c r="C8" s="207"/>
-      <c r="D8" s="200"/>
-      <c r="E8" s="201"/>
-      <c r="F8" s="211"/>
-      <c r="G8" s="172"/>
+      <c r="B8" s="156"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="150"/>
+      <c r="E8" s="151"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="173"/>
       <c r="H8" s="47" t="str">
         <f t="shared" ref="H8:AM8" si="2">IF(MOD(WEEKDAY(H7)+5,7)=0,"Ma",IF(MOD(WEEKDAY(H7)+5,7)=1,"Ti",IF(MOD(WEEKDAY(H7)+5,7)=2,"Ke",IF(MOD(WEEKDAY(H7)+5,7)=3,"To",IF(MOD(WEEKDAY(H7)+5,7)=4,"Pe",IF(MOD(WEEKDAY(H7)+5,7)=5,"La","Su"))))))</f>
         <v>Pe</v>
@@ -5706,11 +6163,11 @@
       <c r="AP8" s="27"/>
     </row>
     <row r="9" spans="2:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="208"/>
-      <c r="C9" s="209"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="203"/>
-      <c r="F9" s="212"/>
+      <c r="B9" s="158"/>
+      <c r="C9" s="159"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="153"/>
+      <c r="F9" s="162"/>
       <c r="G9" s="50"/>
       <c r="H9" s="51"/>
       <c r="I9" s="51"/>
@@ -5749,15 +6206,15 @@
       <c r="AP9" s="27"/>
     </row>
     <row r="10" spans="2:43" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="156">
+      <c r="B10" s="140">
         <v>1214</v>
       </c>
-      <c r="C10" s="157"/>
-      <c r="D10" s="162" t="s">
+      <c r="C10" s="163"/>
+      <c r="D10" s="174" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="157"/>
-      <c r="F10" s="173">
+      <c r="E10" s="163"/>
+      <c r="F10" s="178">
         <v>333555</v>
       </c>
       <c r="G10" s="57" t="s">
@@ -5817,11 +6274,11 @@
       <c r="AQ10" s="34"/>
     </row>
     <row r="11" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="158"/>
-      <c r="C11" s="159"/>
-      <c r="D11" s="163"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="174"/>
+      <c r="B11" s="164"/>
+      <c r="C11" s="165"/>
+      <c r="D11" s="175"/>
+      <c r="E11" s="165"/>
+      <c r="F11" s="179"/>
       <c r="G11" s="60" t="s">
         <v>15</v>
       </c>
@@ -5863,11 +6320,11 @@
       <c r="AQ11" s="34"/>
     </row>
     <row r="12" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="158"/>
-      <c r="C12" s="159"/>
-      <c r="D12" s="163"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="174"/>
+      <c r="B12" s="164"/>
+      <c r="C12" s="165"/>
+      <c r="D12" s="175"/>
+      <c r="E12" s="165"/>
+      <c r="F12" s="179"/>
       <c r="G12" s="63" t="s">
         <v>16</v>
       </c>
@@ -5909,11 +6366,11 @@
       <c r="AQ12" s="34"/>
     </row>
     <row r="13" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="158"/>
-      <c r="C13" s="159"/>
-      <c r="D13" s="163"/>
-      <c r="E13" s="159"/>
-      <c r="F13" s="174"/>
+      <c r="B13" s="164"/>
+      <c r="C13" s="165"/>
+      <c r="D13" s="175"/>
+      <c r="E13" s="165"/>
+      <c r="F13" s="179"/>
       <c r="G13" s="63" t="s">
         <v>17</v>
       </c>
@@ -5955,11 +6412,11 @@
       <c r="AQ13" s="34"/>
     </row>
     <row r="14" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="158"/>
-      <c r="C14" s="159"/>
-      <c r="D14" s="163"/>
-      <c r="E14" s="159"/>
-      <c r="F14" s="174"/>
+      <c r="B14" s="164"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="179"/>
       <c r="G14" s="63" t="s">
         <v>18</v>
       </c>
@@ -6001,11 +6458,11 @@
       <c r="AQ14" s="34"/>
     </row>
     <row r="15" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="158"/>
-      <c r="C15" s="159"/>
-      <c r="D15" s="163"/>
-      <c r="E15" s="159"/>
-      <c r="F15" s="174"/>
+      <c r="B15" s="164"/>
+      <c r="C15" s="165"/>
+      <c r="D15" s="175"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="179"/>
       <c r="G15" s="63" t="s">
         <v>19</v>
       </c>
@@ -6047,11 +6504,11 @@
       <c r="AQ15" s="34"/>
     </row>
     <row r="16" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="158"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="163"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="174"/>
+      <c r="B16" s="164"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="175"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="179"/>
       <c r="G16" s="69" t="s">
         <v>20</v>
       </c>
@@ -6093,11 +6550,11 @@
       <c r="AQ16" s="34"/>
     </row>
     <row r="17" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="158"/>
-      <c r="C17" s="159"/>
-      <c r="D17" s="164"/>
-      <c r="E17" s="159"/>
-      <c r="F17" s="174"/>
+      <c r="B17" s="164"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="176"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="179"/>
       <c r="G17" s="63" t="s">
         <v>30</v>
       </c>
@@ -6139,11 +6596,11 @@
       <c r="AQ17" s="34"/>
     </row>
     <row r="18" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="158"/>
-      <c r="C18" s="159"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="174"/>
+      <c r="B18" s="164"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="176"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="179"/>
       <c r="G18" s="63" t="s">
         <v>23</v>
       </c>
@@ -6185,11 +6642,11 @@
       <c r="AQ18" s="34"/>
     </row>
     <row r="19" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="158"/>
-      <c r="C19" s="159"/>
-      <c r="D19" s="164"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="174"/>
+      <c r="B19" s="164"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="176"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="179"/>
       <c r="G19" s="63" t="s">
         <v>26</v>
       </c>
@@ -6231,11 +6688,11 @@
       <c r="AQ19" s="34"/>
     </row>
     <row r="20" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="158"/>
-      <c r="C20" s="159"/>
-      <c r="D20" s="164"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="174"/>
+      <c r="B20" s="164"/>
+      <c r="C20" s="165"/>
+      <c r="D20" s="176"/>
+      <c r="E20" s="165"/>
+      <c r="F20" s="179"/>
       <c r="G20" s="63" t="s">
         <v>24</v>
       </c>
@@ -6277,11 +6734,11 @@
       <c r="AQ20" s="34"/>
     </row>
     <row r="21" spans="2:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="160"/>
-      <c r="C21" s="161"/>
-      <c r="D21" s="165"/>
-      <c r="E21" s="161"/>
-      <c r="F21" s="175"/>
+      <c r="B21" s="166"/>
+      <c r="C21" s="167"/>
+      <c r="D21" s="177"/>
+      <c r="E21" s="167"/>
+      <c r="F21" s="180"/>
       <c r="G21" s="70" t="s">
         <v>25</v>
       </c>
@@ -6323,15 +6780,15 @@
       <c r="AQ21" s="34"/>
     </row>
     <row r="22" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="156">
+      <c r="B22" s="140">
         <v>5555</v>
       </c>
-      <c r="C22" s="176"/>
-      <c r="D22" s="162" t="s">
+      <c r="C22" s="141"/>
+      <c r="D22" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="157"/>
-      <c r="F22" s="173">
+      <c r="E22" s="163"/>
+      <c r="F22" s="178">
         <v>667333</v>
       </c>
       <c r="G22" s="57" t="s">
@@ -6395,11 +6852,11 @@
       <c r="AQ22" s="34"/>
     </row>
     <row r="23" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="194"/>
-      <c r="C23" s="178"/>
-      <c r="D23" s="163"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="183"/>
+      <c r="B23" s="142"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="175"/>
+      <c r="E23" s="165"/>
+      <c r="F23" s="186"/>
       <c r="G23" s="60" t="s">
         <v>15</v>
       </c>
@@ -6441,11 +6898,11 @@
       <c r="AQ23" s="34"/>
     </row>
     <row r="24" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="194"/>
-      <c r="C24" s="178"/>
-      <c r="D24" s="163"/>
-      <c r="E24" s="159"/>
-      <c r="F24" s="183"/>
+      <c r="B24" s="142"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="175"/>
+      <c r="E24" s="165"/>
+      <c r="F24" s="186"/>
       <c r="G24" s="63" t="s">
         <v>16</v>
       </c>
@@ -6487,11 +6944,11 @@
       <c r="AQ24" s="34"/>
     </row>
     <row r="25" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="194"/>
-      <c r="C25" s="178"/>
-      <c r="D25" s="163"/>
-      <c r="E25" s="159"/>
-      <c r="F25" s="183"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="143"/>
+      <c r="D25" s="175"/>
+      <c r="E25" s="165"/>
+      <c r="F25" s="186"/>
       <c r="G25" s="63" t="s">
         <v>17</v>
       </c>
@@ -6533,11 +6990,11 @@
       <c r="AQ25" s="34"/>
     </row>
     <row r="26" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="194"/>
-      <c r="C26" s="178"/>
-      <c r="D26" s="163"/>
-      <c r="E26" s="159"/>
-      <c r="F26" s="183"/>
+      <c r="B26" s="142"/>
+      <c r="C26" s="143"/>
+      <c r="D26" s="175"/>
+      <c r="E26" s="165"/>
+      <c r="F26" s="186"/>
       <c r="G26" s="63" t="s">
         <v>18</v>
       </c>
@@ -6579,11 +7036,11 @@
       <c r="AQ26" s="34"/>
     </row>
     <row r="27" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="194"/>
-      <c r="C27" s="178"/>
-      <c r="D27" s="163"/>
-      <c r="E27" s="159"/>
-      <c r="F27" s="183"/>
+      <c r="B27" s="142"/>
+      <c r="C27" s="143"/>
+      <c r="D27" s="175"/>
+      <c r="E27" s="165"/>
+      <c r="F27" s="186"/>
       <c r="G27" s="63" t="s">
         <v>19</v>
       </c>
@@ -6625,11 +7082,11 @@
       <c r="AQ27" s="34"/>
     </row>
     <row r="28" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="194"/>
-      <c r="C28" s="178"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="159"/>
-      <c r="F28" s="183"/>
+      <c r="B28" s="142"/>
+      <c r="C28" s="143"/>
+      <c r="D28" s="175"/>
+      <c r="E28" s="165"/>
+      <c r="F28" s="186"/>
       <c r="G28" s="69" t="s">
         <v>20</v>
       </c>
@@ -6671,11 +7128,11 @@
       <c r="AQ28" s="34"/>
     </row>
     <row r="29" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="194"/>
-      <c r="C29" s="178"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="183"/>
+      <c r="B29" s="142"/>
+      <c r="C29" s="143"/>
+      <c r="D29" s="176"/>
+      <c r="E29" s="165"/>
+      <c r="F29" s="186"/>
       <c r="G29" s="63" t="s">
         <v>30</v>
       </c>
@@ -6717,11 +7174,11 @@
       <c r="AQ29" s="34"/>
     </row>
     <row r="30" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="194"/>
-      <c r="C30" s="178"/>
-      <c r="D30" s="164"/>
-      <c r="E30" s="159"/>
-      <c r="F30" s="183"/>
+      <c r="B30" s="142"/>
+      <c r="C30" s="143"/>
+      <c r="D30" s="176"/>
+      <c r="E30" s="165"/>
+      <c r="F30" s="186"/>
       <c r="G30" s="63" t="s">
         <v>23</v>
       </c>
@@ -6773,11 +7230,11 @@
       <c r="AQ30" s="34"/>
     </row>
     <row r="31" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="194"/>
-      <c r="C31" s="178"/>
-      <c r="D31" s="164"/>
-      <c r="E31" s="159"/>
-      <c r="F31" s="183"/>
+      <c r="B31" s="142"/>
+      <c r="C31" s="143"/>
+      <c r="D31" s="176"/>
+      <c r="E31" s="165"/>
+      <c r="F31" s="186"/>
       <c r="G31" s="63" t="s">
         <v>26</v>
       </c>
@@ -6829,11 +7286,11 @@
       <c r="AQ31" s="34"/>
     </row>
     <row r="32" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="194"/>
-      <c r="C32" s="178"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="159"/>
-      <c r="F32" s="183"/>
+      <c r="B32" s="142"/>
+      <c r="C32" s="143"/>
+      <c r="D32" s="176"/>
+      <c r="E32" s="165"/>
+      <c r="F32" s="186"/>
       <c r="G32" s="63" t="s">
         <v>24</v>
       </c>
@@ -6875,11 +7332,11 @@
       <c r="AQ32" s="34"/>
     </row>
     <row r="33" spans="2:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="195"/>
-      <c r="C33" s="180"/>
-      <c r="D33" s="165"/>
-      <c r="E33" s="161"/>
-      <c r="F33" s="184"/>
+      <c r="B33" s="144"/>
+      <c r="C33" s="145"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="167"/>
+      <c r="F33" s="187"/>
       <c r="G33" s="70" t="s">
         <v>25</v>
       </c>
@@ -6921,15 +7378,15 @@
       <c r="AQ33" s="34"/>
     </row>
     <row r="34" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="156">
+      <c r="B34" s="140">
         <v>9000</v>
       </c>
-      <c r="C34" s="176"/>
-      <c r="D34" s="162" t="s">
+      <c r="C34" s="141"/>
+      <c r="D34" s="174" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="176"/>
-      <c r="F34" s="166"/>
+      <c r="E34" s="141"/>
+      <c r="F34" s="183"/>
       <c r="G34" s="57" t="s">
         <v>27</v>
       </c>
@@ -6977,11 +7434,11 @@
       <c r="AQ34" s="34"/>
     </row>
     <row r="35" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="194"/>
-      <c r="C35" s="178"/>
-      <c r="D35" s="177"/>
-      <c r="E35" s="178"/>
-      <c r="F35" s="181"/>
+      <c r="B35" s="142"/>
+      <c r="C35" s="143"/>
+      <c r="D35" s="181"/>
+      <c r="E35" s="143"/>
+      <c r="F35" s="184"/>
       <c r="G35" s="60" t="s">
         <v>15</v>
       </c>
@@ -7023,11 +7480,11 @@
       <c r="AQ35" s="34"/>
     </row>
     <row r="36" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="194"/>
-      <c r="C36" s="178"/>
-      <c r="D36" s="177"/>
-      <c r="E36" s="178"/>
-      <c r="F36" s="181"/>
+      <c r="B36" s="142"/>
+      <c r="C36" s="143"/>
+      <c r="D36" s="181"/>
+      <c r="E36" s="143"/>
+      <c r="F36" s="184"/>
       <c r="G36" s="63" t="s">
         <v>16</v>
       </c>
@@ -7072,11 +7529,11 @@
       <c r="AQ36" s="34"/>
     </row>
     <row r="37" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="194"/>
-      <c r="C37" s="178"/>
-      <c r="D37" s="177"/>
-      <c r="E37" s="178"/>
-      <c r="F37" s="181"/>
+      <c r="B37" s="142"/>
+      <c r="C37" s="143"/>
+      <c r="D37" s="181"/>
+      <c r="E37" s="143"/>
+      <c r="F37" s="184"/>
       <c r="G37" s="63" t="s">
         <v>17</v>
       </c>
@@ -7121,11 +7578,11 @@
       <c r="AQ37" s="34"/>
     </row>
     <row r="38" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="194"/>
-      <c r="C38" s="178"/>
-      <c r="D38" s="177"/>
-      <c r="E38" s="178"/>
-      <c r="F38" s="181"/>
+      <c r="B38" s="142"/>
+      <c r="C38" s="143"/>
+      <c r="D38" s="181"/>
+      <c r="E38" s="143"/>
+      <c r="F38" s="184"/>
       <c r="G38" s="63" t="s">
         <v>18</v>
       </c>
@@ -7170,11 +7627,11 @@
       <c r="AQ38" s="34"/>
     </row>
     <row r="39" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="194"/>
-      <c r="C39" s="178"/>
-      <c r="D39" s="177"/>
-      <c r="E39" s="178"/>
-      <c r="F39" s="181"/>
+      <c r="B39" s="142"/>
+      <c r="C39" s="143"/>
+      <c r="D39" s="181"/>
+      <c r="E39" s="143"/>
+      <c r="F39" s="184"/>
       <c r="G39" s="63" t="s">
         <v>19</v>
       </c>
@@ -7219,11 +7676,11 @@
       <c r="AQ39" s="34"/>
     </row>
     <row r="40" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="194"/>
-      <c r="C40" s="178"/>
-      <c r="D40" s="177"/>
-      <c r="E40" s="178"/>
-      <c r="F40" s="181"/>
+      <c r="B40" s="142"/>
+      <c r="C40" s="143"/>
+      <c r="D40" s="181"/>
+      <c r="E40" s="143"/>
+      <c r="F40" s="184"/>
       <c r="G40" s="69" t="s">
         <v>20</v>
       </c>
@@ -7268,11 +7725,11 @@
       <c r="AQ40" s="34"/>
     </row>
     <row r="41" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="194"/>
-      <c r="C41" s="178"/>
-      <c r="D41" s="177"/>
-      <c r="E41" s="178"/>
-      <c r="F41" s="181"/>
+      <c r="B41" s="142"/>
+      <c r="C41" s="143"/>
+      <c r="D41" s="181"/>
+      <c r="E41" s="143"/>
+      <c r="F41" s="184"/>
       <c r="G41" s="63" t="s">
         <v>30</v>
       </c>
@@ -7317,11 +7774,11 @@
       <c r="AQ41" s="34"/>
     </row>
     <row r="42" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="194"/>
-      <c r="C42" s="178"/>
-      <c r="D42" s="177"/>
-      <c r="E42" s="178"/>
-      <c r="F42" s="181"/>
+      <c r="B42" s="142"/>
+      <c r="C42" s="143"/>
+      <c r="D42" s="181"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="184"/>
       <c r="G42" s="63" t="s">
         <v>23</v>
       </c>
@@ -7366,11 +7823,11 @@
       <c r="AQ42" s="34"/>
     </row>
     <row r="43" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="194"/>
-      <c r="C43" s="178"/>
-      <c r="D43" s="177"/>
-      <c r="E43" s="178"/>
-      <c r="F43" s="181"/>
+      <c r="B43" s="142"/>
+      <c r="C43" s="143"/>
+      <c r="D43" s="181"/>
+      <c r="E43" s="143"/>
+      <c r="F43" s="184"/>
       <c r="G43" s="63" t="s">
         <v>26</v>
       </c>
@@ -7415,11 +7872,11 @@
       <c r="AQ43" s="34"/>
     </row>
     <row r="44" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="194"/>
-      <c r="C44" s="178"/>
-      <c r="D44" s="177"/>
-      <c r="E44" s="178"/>
-      <c r="F44" s="181"/>
+      <c r="B44" s="142"/>
+      <c r="C44" s="143"/>
+      <c r="D44" s="181"/>
+      <c r="E44" s="143"/>
+      <c r="F44" s="184"/>
       <c r="G44" s="63" t="s">
         <v>24</v>
       </c>
@@ -7464,11 +7921,11 @@
       <c r="AQ44" s="34"/>
     </row>
     <row r="45" spans="2:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="195"/>
-      <c r="C45" s="180"/>
-      <c r="D45" s="179"/>
-      <c r="E45" s="180"/>
-      <c r="F45" s="182"/>
+      <c r="B45" s="144"/>
+      <c r="C45" s="145"/>
+      <c r="D45" s="182"/>
+      <c r="E45" s="145"/>
+      <c r="F45" s="185"/>
       <c r="G45" s="70" t="s">
         <v>25</v>
       </c>
@@ -7513,11 +7970,11 @@
       <c r="AQ45" s="34"/>
     </row>
     <row r="46" spans="2:43" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="156"/>
-      <c r="C46" s="176"/>
-      <c r="D46" s="162"/>
-      <c r="E46" s="176"/>
-      <c r="F46" s="166"/>
+      <c r="B46" s="140"/>
+      <c r="C46" s="141"/>
+      <c r="D46" s="174"/>
+      <c r="E46" s="141"/>
+      <c r="F46" s="183"/>
       <c r="G46" s="57" t="s">
         <v>27</v>
       </c>
@@ -7562,11 +8019,11 @@
       <c r="AQ46" s="34"/>
     </row>
     <row r="47" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="194"/>
-      <c r="C47" s="178"/>
-      <c r="D47" s="177"/>
-      <c r="E47" s="178"/>
-      <c r="F47" s="181"/>
+      <c r="B47" s="142"/>
+      <c r="C47" s="143"/>
+      <c r="D47" s="181"/>
+      <c r="E47" s="143"/>
+      <c r="F47" s="184"/>
       <c r="G47" s="60" t="s">
         <v>15</v>
       </c>
@@ -7611,11 +8068,11 @@
       <c r="AQ47" s="34"/>
     </row>
     <row r="48" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="194"/>
-      <c r="C48" s="178"/>
-      <c r="D48" s="177"/>
-      <c r="E48" s="178"/>
-      <c r="F48" s="181"/>
+      <c r="B48" s="142"/>
+      <c r="C48" s="143"/>
+      <c r="D48" s="181"/>
+      <c r="E48" s="143"/>
+      <c r="F48" s="184"/>
       <c r="G48" s="63" t="s">
         <v>16</v>
       </c>
@@ -7660,11 +8117,11 @@
       <c r="AQ48" s="34"/>
     </row>
     <row r="49" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="194"/>
-      <c r="C49" s="178"/>
-      <c r="D49" s="177"/>
-      <c r="E49" s="178"/>
-      <c r="F49" s="181"/>
+      <c r="B49" s="142"/>
+      <c r="C49" s="143"/>
+      <c r="D49" s="181"/>
+      <c r="E49" s="143"/>
+      <c r="F49" s="184"/>
       <c r="G49" s="63" t="s">
         <v>17</v>
       </c>
@@ -7709,11 +8166,11 @@
       <c r="AQ49" s="34"/>
     </row>
     <row r="50" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="194"/>
-      <c r="C50" s="178"/>
-      <c r="D50" s="177"/>
-      <c r="E50" s="178"/>
-      <c r="F50" s="181"/>
+      <c r="B50" s="142"/>
+      <c r="C50" s="143"/>
+      <c r="D50" s="181"/>
+      <c r="E50" s="143"/>
+      <c r="F50" s="184"/>
       <c r="G50" s="63" t="s">
         <v>18</v>
       </c>
@@ -7758,11 +8215,11 @@
       <c r="AQ50" s="34"/>
     </row>
     <row r="51" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="194"/>
-      <c r="C51" s="178"/>
-      <c r="D51" s="177"/>
-      <c r="E51" s="178"/>
-      <c r="F51" s="181"/>
+      <c r="B51" s="142"/>
+      <c r="C51" s="143"/>
+      <c r="D51" s="181"/>
+      <c r="E51" s="143"/>
+      <c r="F51" s="184"/>
       <c r="G51" s="63" t="s">
         <v>19</v>
       </c>
@@ -7807,11 +8264,11 @@
       <c r="AQ51" s="34"/>
     </row>
     <row r="52" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="194"/>
-      <c r="C52" s="178"/>
-      <c r="D52" s="177"/>
-      <c r="E52" s="178"/>
-      <c r="F52" s="181"/>
+      <c r="B52" s="142"/>
+      <c r="C52" s="143"/>
+      <c r="D52" s="181"/>
+      <c r="E52" s="143"/>
+      <c r="F52" s="184"/>
       <c r="G52" s="69" t="s">
         <v>20</v>
       </c>
@@ -7856,11 +8313,11 @@
       <c r="AQ52" s="34"/>
     </row>
     <row r="53" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="194"/>
-      <c r="C53" s="178"/>
-      <c r="D53" s="177"/>
-      <c r="E53" s="178"/>
-      <c r="F53" s="181"/>
+      <c r="B53" s="142"/>
+      <c r="C53" s="143"/>
+      <c r="D53" s="181"/>
+      <c r="E53" s="143"/>
+      <c r="F53" s="184"/>
       <c r="G53" s="63" t="s">
         <v>30</v>
       </c>
@@ -7905,11 +8362,11 @@
       <c r="AQ53" s="34"/>
     </row>
     <row r="54" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="194"/>
-      <c r="C54" s="178"/>
-      <c r="D54" s="177"/>
-      <c r="E54" s="178"/>
-      <c r="F54" s="181"/>
+      <c r="B54" s="142"/>
+      <c r="C54" s="143"/>
+      <c r="D54" s="181"/>
+      <c r="E54" s="143"/>
+      <c r="F54" s="184"/>
       <c r="G54" s="63" t="s">
         <v>23</v>
       </c>
@@ -7954,11 +8411,11 @@
       <c r="AQ54" s="34"/>
     </row>
     <row r="55" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="194"/>
-      <c r="C55" s="178"/>
-      <c r="D55" s="177"/>
-      <c r="E55" s="178"/>
-      <c r="F55" s="181"/>
+      <c r="B55" s="142"/>
+      <c r="C55" s="143"/>
+      <c r="D55" s="181"/>
+      <c r="E55" s="143"/>
+      <c r="F55" s="184"/>
       <c r="G55" s="63" t="s">
         <v>26</v>
       </c>
@@ -8003,11 +8460,11 @@
       <c r="AQ55" s="34"/>
     </row>
     <row r="56" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="194"/>
-      <c r="C56" s="178"/>
-      <c r="D56" s="177"/>
-      <c r="E56" s="178"/>
-      <c r="F56" s="181"/>
+      <c r="B56" s="142"/>
+      <c r="C56" s="143"/>
+      <c r="D56" s="181"/>
+      <c r="E56" s="143"/>
+      <c r="F56" s="184"/>
       <c r="G56" s="63" t="s">
         <v>24</v>
       </c>
@@ -8052,11 +8509,11 @@
       <c r="AQ56" s="34"/>
     </row>
     <row r="57" spans="2:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="195"/>
-      <c r="C57" s="180"/>
-      <c r="D57" s="179"/>
-      <c r="E57" s="180"/>
-      <c r="F57" s="182"/>
+      <c r="B57" s="144"/>
+      <c r="C57" s="145"/>
+      <c r="D57" s="182"/>
+      <c r="E57" s="145"/>
+      <c r="F57" s="185"/>
       <c r="G57" s="70" t="s">
         <v>25</v>
       </c>
@@ -8101,11 +8558,11 @@
       <c r="AQ57" s="34"/>
     </row>
     <row r="58" spans="2:43" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="156"/>
-      <c r="C58" s="157"/>
-      <c r="D58" s="162"/>
-      <c r="E58" s="157"/>
-      <c r="F58" s="147"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="163"/>
+      <c r="D58" s="174"/>
+      <c r="E58" s="163"/>
+      <c r="F58" s="190"/>
       <c r="G58" s="57" t="s">
         <v>27</v>
       </c>
@@ -8150,11 +8607,11 @@
       <c r="AQ58" s="34"/>
     </row>
     <row r="59" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="158"/>
-      <c r="C59" s="159"/>
-      <c r="D59" s="163"/>
-      <c r="E59" s="159"/>
-      <c r="F59" s="148"/>
+      <c r="B59" s="164"/>
+      <c r="C59" s="165"/>
+      <c r="D59" s="175"/>
+      <c r="E59" s="165"/>
+      <c r="F59" s="191"/>
       <c r="G59" s="60" t="s">
         <v>15</v>
       </c>
@@ -8199,11 +8656,11 @@
       <c r="AQ59" s="34"/>
     </row>
     <row r="60" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="158"/>
-      <c r="C60" s="159"/>
-      <c r="D60" s="163"/>
-      <c r="E60" s="159"/>
-      <c r="F60" s="148"/>
+      <c r="B60" s="164"/>
+      <c r="C60" s="165"/>
+      <c r="D60" s="175"/>
+      <c r="E60" s="165"/>
+      <c r="F60" s="191"/>
       <c r="G60" s="63" t="s">
         <v>16</v>
       </c>
@@ -8248,11 +8705,11 @@
       <c r="AQ60" s="34"/>
     </row>
     <row r="61" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="158"/>
-      <c r="C61" s="159"/>
-      <c r="D61" s="163"/>
-      <c r="E61" s="159"/>
-      <c r="F61" s="148"/>
+      <c r="B61" s="164"/>
+      <c r="C61" s="165"/>
+      <c r="D61" s="175"/>
+      <c r="E61" s="165"/>
+      <c r="F61" s="191"/>
       <c r="G61" s="63" t="s">
         <v>17</v>
       </c>
@@ -8297,11 +8754,11 @@
       <c r="AQ61" s="34"/>
     </row>
     <row r="62" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="158"/>
-      <c r="C62" s="159"/>
-      <c r="D62" s="163"/>
-      <c r="E62" s="159"/>
-      <c r="F62" s="148"/>
+      <c r="B62" s="164"/>
+      <c r="C62" s="165"/>
+      <c r="D62" s="175"/>
+      <c r="E62" s="165"/>
+      <c r="F62" s="191"/>
       <c r="G62" s="63" t="s">
         <v>18</v>
       </c>
@@ -8346,11 +8803,11 @@
       <c r="AQ62" s="34"/>
     </row>
     <row r="63" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="158"/>
-      <c r="C63" s="159"/>
-      <c r="D63" s="163"/>
-      <c r="E63" s="159"/>
-      <c r="F63" s="148"/>
+      <c r="B63" s="164"/>
+      <c r="C63" s="165"/>
+      <c r="D63" s="175"/>
+      <c r="E63" s="165"/>
+      <c r="F63" s="191"/>
       <c r="G63" s="63" t="s">
         <v>19</v>
       </c>
@@ -8395,11 +8852,11 @@
       <c r="AQ63" s="34"/>
     </row>
     <row r="64" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="158"/>
-      <c r="C64" s="159"/>
-      <c r="D64" s="163"/>
-      <c r="E64" s="159"/>
-      <c r="F64" s="148"/>
+      <c r="B64" s="164"/>
+      <c r="C64" s="165"/>
+      <c r="D64" s="175"/>
+      <c r="E64" s="165"/>
+      <c r="F64" s="191"/>
       <c r="G64" s="69" t="s">
         <v>20</v>
       </c>
@@ -8444,11 +8901,11 @@
       <c r="AQ64" s="34"/>
     </row>
     <row r="65" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="158"/>
-      <c r="C65" s="159"/>
-      <c r="D65" s="164"/>
-      <c r="E65" s="159"/>
-      <c r="F65" s="148"/>
+      <c r="B65" s="164"/>
+      <c r="C65" s="165"/>
+      <c r="D65" s="176"/>
+      <c r="E65" s="165"/>
+      <c r="F65" s="191"/>
       <c r="G65" s="63" t="s">
         <v>30</v>
       </c>
@@ -8493,11 +8950,11 @@
       <c r="AQ65" s="34"/>
     </row>
     <row r="66" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="158"/>
-      <c r="C66" s="159"/>
-      <c r="D66" s="164"/>
-      <c r="E66" s="159"/>
-      <c r="F66" s="148"/>
+      <c r="B66" s="164"/>
+      <c r="C66" s="165"/>
+      <c r="D66" s="176"/>
+      <c r="E66" s="165"/>
+      <c r="F66" s="191"/>
       <c r="G66" s="63" t="s">
         <v>23</v>
       </c>
@@ -8542,11 +8999,11 @@
       <c r="AQ66" s="34"/>
     </row>
     <row r="67" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="158"/>
-      <c r="C67" s="159"/>
-      <c r="D67" s="164"/>
-      <c r="E67" s="159"/>
-      <c r="F67" s="148"/>
+      <c r="B67" s="164"/>
+      <c r="C67" s="165"/>
+      <c r="D67" s="176"/>
+      <c r="E67" s="165"/>
+      <c r="F67" s="191"/>
       <c r="G67" s="63" t="s">
         <v>26</v>
       </c>
@@ -8591,11 +9048,11 @@
       <c r="AQ67" s="34"/>
     </row>
     <row r="68" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="158"/>
-      <c r="C68" s="159"/>
-      <c r="D68" s="164"/>
-      <c r="E68" s="159"/>
-      <c r="F68" s="148"/>
+      <c r="B68" s="164"/>
+      <c r="C68" s="165"/>
+      <c r="D68" s="176"/>
+      <c r="E68" s="165"/>
+      <c r="F68" s="191"/>
       <c r="G68" s="63" t="s">
         <v>24</v>
       </c>
@@ -8640,11 +9097,11 @@
       <c r="AQ68" s="34"/>
     </row>
     <row r="69" spans="2:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="160"/>
-      <c r="C69" s="161"/>
-      <c r="D69" s="165"/>
-      <c r="E69" s="161"/>
-      <c r="F69" s="149"/>
+      <c r="B69" s="166"/>
+      <c r="C69" s="167"/>
+      <c r="D69" s="177"/>
+      <c r="E69" s="167"/>
+      <c r="F69" s="192"/>
       <c r="G69" s="70" t="s">
         <v>25</v>
       </c>
@@ -8689,11 +9146,11 @@
       <c r="AQ69" s="34"/>
     </row>
     <row r="70" spans="2:43" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="156"/>
-      <c r="C70" s="157"/>
-      <c r="D70" s="162"/>
-      <c r="E70" s="157"/>
-      <c r="F70" s="166"/>
+      <c r="B70" s="140"/>
+      <c r="C70" s="163"/>
+      <c r="D70" s="174"/>
+      <c r="E70" s="163"/>
+      <c r="F70" s="183"/>
       <c r="G70" s="57" t="s">
         <v>27</v>
       </c>
@@ -8738,11 +9195,11 @@
       <c r="AQ70" s="34"/>
     </row>
     <row r="71" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="158"/>
-      <c r="C71" s="159"/>
-      <c r="D71" s="163"/>
-      <c r="E71" s="159"/>
-      <c r="F71" s="167"/>
+      <c r="B71" s="164"/>
+      <c r="C71" s="165"/>
+      <c r="D71" s="175"/>
+      <c r="E71" s="165"/>
+      <c r="F71" s="188"/>
       <c r="G71" s="60" t="s">
         <v>15</v>
       </c>
@@ -8787,11 +9244,11 @@
       <c r="AQ71" s="34"/>
     </row>
     <row r="72" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="158"/>
-      <c r="C72" s="159"/>
-      <c r="D72" s="163"/>
-      <c r="E72" s="159"/>
-      <c r="F72" s="167"/>
+      <c r="B72" s="164"/>
+      <c r="C72" s="165"/>
+      <c r="D72" s="175"/>
+      <c r="E72" s="165"/>
+      <c r="F72" s="188"/>
       <c r="G72" s="63" t="s">
         <v>16</v>
       </c>
@@ -8836,11 +9293,11 @@
       <c r="AQ72" s="34"/>
     </row>
     <row r="73" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="158"/>
-      <c r="C73" s="159"/>
-      <c r="D73" s="163"/>
-      <c r="E73" s="159"/>
-      <c r="F73" s="167"/>
+      <c r="B73" s="164"/>
+      <c r="C73" s="165"/>
+      <c r="D73" s="175"/>
+      <c r="E73" s="165"/>
+      <c r="F73" s="188"/>
       <c r="G73" s="63" t="s">
         <v>17</v>
       </c>
@@ -8885,11 +9342,11 @@
       <c r="AQ73" s="34"/>
     </row>
     <row r="74" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="158"/>
-      <c r="C74" s="159"/>
-      <c r="D74" s="163"/>
-      <c r="E74" s="159"/>
-      <c r="F74" s="167"/>
+      <c r="B74" s="164"/>
+      <c r="C74" s="165"/>
+      <c r="D74" s="175"/>
+      <c r="E74" s="165"/>
+      <c r="F74" s="188"/>
       <c r="G74" s="63" t="s">
         <v>18</v>
       </c>
@@ -8934,11 +9391,11 @@
       <c r="AQ74" s="34"/>
     </row>
     <row r="75" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="158"/>
-      <c r="C75" s="159"/>
-      <c r="D75" s="163"/>
-      <c r="E75" s="159"/>
-      <c r="F75" s="167"/>
+      <c r="B75" s="164"/>
+      <c r="C75" s="165"/>
+      <c r="D75" s="175"/>
+      <c r="E75" s="165"/>
+      <c r="F75" s="188"/>
       <c r="G75" s="63" t="s">
         <v>19</v>
       </c>
@@ -8983,11 +9440,11 @@
       <c r="AQ75" s="34"/>
     </row>
     <row r="76" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="158"/>
-      <c r="C76" s="159"/>
-      <c r="D76" s="163"/>
-      <c r="E76" s="159"/>
-      <c r="F76" s="167"/>
+      <c r="B76" s="164"/>
+      <c r="C76" s="165"/>
+      <c r="D76" s="175"/>
+      <c r="E76" s="165"/>
+      <c r="F76" s="188"/>
       <c r="G76" s="69" t="s">
         <v>20</v>
       </c>
@@ -9032,11 +9489,11 @@
       <c r="AQ76" s="34"/>
     </row>
     <row r="77" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="158"/>
-      <c r="C77" s="159"/>
-      <c r="D77" s="164"/>
-      <c r="E77" s="159"/>
-      <c r="F77" s="167"/>
+      <c r="B77" s="164"/>
+      <c r="C77" s="165"/>
+      <c r="D77" s="176"/>
+      <c r="E77" s="165"/>
+      <c r="F77" s="188"/>
       <c r="G77" s="63" t="s">
         <v>30</v>
       </c>
@@ -9081,11 +9538,11 @@
       <c r="AQ77" s="34"/>
     </row>
     <row r="78" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="158"/>
-      <c r="C78" s="159"/>
-      <c r="D78" s="164"/>
-      <c r="E78" s="159"/>
-      <c r="F78" s="167"/>
+      <c r="B78" s="164"/>
+      <c r="C78" s="165"/>
+      <c r="D78" s="176"/>
+      <c r="E78" s="165"/>
+      <c r="F78" s="188"/>
       <c r="G78" s="63" t="s">
         <v>23</v>
       </c>
@@ -9130,11 +9587,11 @@
       <c r="AQ78" s="34"/>
     </row>
     <row r="79" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="158"/>
-      <c r="C79" s="159"/>
-      <c r="D79" s="164"/>
-      <c r="E79" s="159"/>
-      <c r="F79" s="167"/>
+      <c r="B79" s="164"/>
+      <c r="C79" s="165"/>
+      <c r="D79" s="176"/>
+      <c r="E79" s="165"/>
+      <c r="F79" s="188"/>
       <c r="G79" s="63" t="s">
         <v>26</v>
       </c>
@@ -9179,11 +9636,11 @@
       <c r="AQ79" s="34"/>
     </row>
     <row r="80" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="158"/>
-      <c r="C80" s="159"/>
-      <c r="D80" s="164"/>
-      <c r="E80" s="159"/>
-      <c r="F80" s="167"/>
+      <c r="B80" s="164"/>
+      <c r="C80" s="165"/>
+      <c r="D80" s="176"/>
+      <c r="E80" s="165"/>
+      <c r="F80" s="188"/>
       <c r="G80" s="63" t="s">
         <v>24</v>
       </c>
@@ -9228,11 +9685,11 @@
       <c r="AQ80" s="34"/>
     </row>
     <row r="81" spans="2:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="160"/>
-      <c r="C81" s="161"/>
-      <c r="D81" s="165"/>
-      <c r="E81" s="161"/>
-      <c r="F81" s="168"/>
+      <c r="B81" s="166"/>
+      <c r="C81" s="167"/>
+      <c r="D81" s="177"/>
+      <c r="E81" s="167"/>
+      <c r="F81" s="189"/>
       <c r="G81" s="70" t="s">
         <v>25</v>
       </c>
@@ -9277,11 +9734,11 @@
       <c r="AQ81" s="34"/>
     </row>
     <row r="82" spans="2:43" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="156"/>
-      <c r="C82" s="157"/>
-      <c r="D82" s="162"/>
-      <c r="E82" s="157"/>
-      <c r="F82" s="147"/>
+      <c r="B82" s="140"/>
+      <c r="C82" s="163"/>
+      <c r="D82" s="174"/>
+      <c r="E82" s="163"/>
+      <c r="F82" s="190"/>
       <c r="G82" s="57" t="s">
         <v>27</v>
       </c>
@@ -9326,11 +9783,11 @@
       <c r="AQ82" s="34"/>
     </row>
     <row r="83" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="158"/>
-      <c r="C83" s="159"/>
-      <c r="D83" s="163"/>
-      <c r="E83" s="159"/>
-      <c r="F83" s="148"/>
+      <c r="B83" s="164"/>
+      <c r="C83" s="165"/>
+      <c r="D83" s="175"/>
+      <c r="E83" s="165"/>
+      <c r="F83" s="191"/>
       <c r="G83" s="60" t="s">
         <v>15</v>
       </c>
@@ -9375,11 +9832,11 @@
       <c r="AQ83" s="34"/>
     </row>
     <row r="84" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="158"/>
-      <c r="C84" s="159"/>
-      <c r="D84" s="163"/>
-      <c r="E84" s="159"/>
-      <c r="F84" s="148"/>
+      <c r="B84" s="164"/>
+      <c r="C84" s="165"/>
+      <c r="D84" s="175"/>
+      <c r="E84" s="165"/>
+      <c r="F84" s="191"/>
       <c r="G84" s="63" t="s">
         <v>16</v>
       </c>
@@ -9424,11 +9881,11 @@
       <c r="AQ84" s="34"/>
     </row>
     <row r="85" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="158"/>
-      <c r="C85" s="159"/>
-      <c r="D85" s="163"/>
-      <c r="E85" s="159"/>
-      <c r="F85" s="148"/>
+      <c r="B85" s="164"/>
+      <c r="C85" s="165"/>
+      <c r="D85" s="175"/>
+      <c r="E85" s="165"/>
+      <c r="F85" s="191"/>
       <c r="G85" s="63" t="s">
         <v>17</v>
       </c>
@@ -9473,11 +9930,11 @@
       <c r="AQ85" s="34"/>
     </row>
     <row r="86" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="158"/>
-      <c r="C86" s="159"/>
-      <c r="D86" s="163"/>
-      <c r="E86" s="159"/>
-      <c r="F86" s="148"/>
+      <c r="B86" s="164"/>
+      <c r="C86" s="165"/>
+      <c r="D86" s="175"/>
+      <c r="E86" s="165"/>
+      <c r="F86" s="191"/>
       <c r="G86" s="63" t="s">
         <v>18</v>
       </c>
@@ -9522,11 +9979,11 @@
       <c r="AQ86" s="34"/>
     </row>
     <row r="87" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="158"/>
-      <c r="C87" s="159"/>
-      <c r="D87" s="163"/>
-      <c r="E87" s="159"/>
-      <c r="F87" s="148"/>
+      <c r="B87" s="164"/>
+      <c r="C87" s="165"/>
+      <c r="D87" s="175"/>
+      <c r="E87" s="165"/>
+      <c r="F87" s="191"/>
       <c r="G87" s="63" t="s">
         <v>19</v>
       </c>
@@ -9571,11 +10028,11 @@
       <c r="AQ87" s="34"/>
     </row>
     <row r="88" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="158"/>
-      <c r="C88" s="159"/>
-      <c r="D88" s="163"/>
-      <c r="E88" s="159"/>
-      <c r="F88" s="148"/>
+      <c r="B88" s="164"/>
+      <c r="C88" s="165"/>
+      <c r="D88" s="175"/>
+      <c r="E88" s="165"/>
+      <c r="F88" s="191"/>
       <c r="G88" s="69" t="s">
         <v>20</v>
       </c>
@@ -9620,11 +10077,11 @@
       <c r="AQ88" s="127"/>
     </row>
     <row r="89" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="158"/>
-      <c r="C89" s="159"/>
-      <c r="D89" s="164"/>
-      <c r="E89" s="159"/>
-      <c r="F89" s="148"/>
+      <c r="B89" s="164"/>
+      <c r="C89" s="165"/>
+      <c r="D89" s="176"/>
+      <c r="E89" s="165"/>
+      <c r="F89" s="191"/>
       <c r="G89" s="63" t="s">
         <v>30</v>
       </c>
@@ -9669,11 +10126,11 @@
       <c r="AQ89" s="127"/>
     </row>
     <row r="90" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="158"/>
-      <c r="C90" s="159"/>
-      <c r="D90" s="164"/>
-      <c r="E90" s="159"/>
-      <c r="F90" s="148"/>
+      <c r="B90" s="164"/>
+      <c r="C90" s="165"/>
+      <c r="D90" s="176"/>
+      <c r="E90" s="165"/>
+      <c r="F90" s="191"/>
       <c r="G90" s="63" t="s">
         <v>23</v>
       </c>
@@ -9718,11 +10175,11 @@
       <c r="AQ90" s="127"/>
     </row>
     <row r="91" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="158"/>
-      <c r="C91" s="159"/>
-      <c r="D91" s="164"/>
-      <c r="E91" s="159"/>
-      <c r="F91" s="148"/>
+      <c r="B91" s="164"/>
+      <c r="C91" s="165"/>
+      <c r="D91" s="176"/>
+      <c r="E91" s="165"/>
+      <c r="F91" s="191"/>
       <c r="G91" s="63" t="s">
         <v>26</v>
       </c>
@@ -9767,11 +10224,11 @@
       <c r="AQ91" s="34"/>
     </row>
     <row r="92" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="158"/>
-      <c r="C92" s="159"/>
-      <c r="D92" s="164"/>
-      <c r="E92" s="159"/>
-      <c r="F92" s="148"/>
+      <c r="B92" s="164"/>
+      <c r="C92" s="165"/>
+      <c r="D92" s="176"/>
+      <c r="E92" s="165"/>
+      <c r="F92" s="191"/>
       <c r="G92" s="63" t="s">
         <v>24</v>
       </c>
@@ -9815,11 +10272,11 @@
       <c r="AP92" s="27"/>
     </row>
     <row r="93" spans="2:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="160"/>
-      <c r="C93" s="161"/>
-      <c r="D93" s="165"/>
-      <c r="E93" s="161"/>
-      <c r="F93" s="149"/>
+      <c r="B93" s="166"/>
+      <c r="C93" s="167"/>
+      <c r="D93" s="177"/>
+      <c r="E93" s="167"/>
+      <c r="F93" s="192"/>
       <c r="G93" s="70" t="s">
         <v>25</v>
       </c>
@@ -9863,13 +10320,13 @@
       <c r="AP93" s="27"/>
     </row>
     <row r="94" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="150"/>
-      <c r="C94" s="151"/>
-      <c r="D94" s="169" t="s">
+      <c r="B94" s="206"/>
+      <c r="C94" s="207"/>
+      <c r="D94" s="212" t="s">
         <v>33</v>
       </c>
-      <c r="E94" s="151"/>
-      <c r="F94" s="185"/>
+      <c r="E94" s="207"/>
+      <c r="F94" s="215"/>
       <c r="G94" s="86" t="s">
         <v>27</v>
       </c>
@@ -10006,11 +10463,11 @@
       <c r="AP94" s="27"/>
     </row>
     <row r="95" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="152"/>
-      <c r="C95" s="153"/>
-      <c r="D95" s="170"/>
-      <c r="E95" s="153"/>
-      <c r="F95" s="186"/>
+      <c r="B95" s="208"/>
+      <c r="C95" s="209"/>
+      <c r="D95" s="213"/>
+      <c r="E95" s="209"/>
+      <c r="F95" s="216"/>
       <c r="G95" s="90" t="s">
         <v>15</v>
       </c>
@@ -10147,11 +10604,11 @@
       <c r="AP95" s="27"/>
     </row>
     <row r="96" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="152"/>
-      <c r="C96" s="153"/>
-      <c r="D96" s="170"/>
-      <c r="E96" s="153"/>
-      <c r="F96" s="186"/>
+      <c r="B96" s="208"/>
+      <c r="C96" s="209"/>
+      <c r="D96" s="213"/>
+      <c r="E96" s="209"/>
+      <c r="F96" s="216"/>
       <c r="G96" s="94" t="s">
         <v>16</v>
       </c>
@@ -10288,11 +10745,11 @@
       <c r="AP96" s="27"/>
     </row>
     <row r="97" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="152"/>
-      <c r="C97" s="153"/>
-      <c r="D97" s="170"/>
-      <c r="E97" s="153"/>
-      <c r="F97" s="186"/>
+      <c r="B97" s="208"/>
+      <c r="C97" s="209"/>
+      <c r="D97" s="213"/>
+      <c r="E97" s="209"/>
+      <c r="F97" s="216"/>
       <c r="G97" s="94" t="s">
         <v>17</v>
       </c>
@@ -10429,11 +10886,11 @@
       <c r="AP97" s="27"/>
     </row>
     <row r="98" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="152"/>
-      <c r="C98" s="153"/>
-      <c r="D98" s="170"/>
-      <c r="E98" s="153"/>
-      <c r="F98" s="186"/>
+      <c r="B98" s="208"/>
+      <c r="C98" s="209"/>
+      <c r="D98" s="213"/>
+      <c r="E98" s="209"/>
+      <c r="F98" s="216"/>
       <c r="G98" s="94" t="s">
         <v>18</v>
       </c>
@@ -10570,11 +11027,11 @@
       <c r="AP98" s="27"/>
     </row>
     <row r="99" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="152"/>
-      <c r="C99" s="153"/>
-      <c r="D99" s="170"/>
-      <c r="E99" s="153"/>
-      <c r="F99" s="186"/>
+      <c r="B99" s="208"/>
+      <c r="C99" s="209"/>
+      <c r="D99" s="213"/>
+      <c r="E99" s="209"/>
+      <c r="F99" s="216"/>
       <c r="G99" s="94" t="s">
         <v>19</v>
       </c>
@@ -10711,11 +11168,11 @@
       <c r="AP99" s="27"/>
     </row>
     <row r="100" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="152"/>
-      <c r="C100" s="153"/>
-      <c r="D100" s="170"/>
-      <c r="E100" s="153"/>
-      <c r="F100" s="186"/>
+      <c r="B100" s="208"/>
+      <c r="C100" s="209"/>
+      <c r="D100" s="213"/>
+      <c r="E100" s="209"/>
+      <c r="F100" s="216"/>
       <c r="G100" s="97" t="s">
         <v>20</v>
       </c>
@@ -10852,11 +11309,11 @@
       <c r="AP100" s="27"/>
     </row>
     <row r="101" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="152"/>
-      <c r="C101" s="153"/>
-      <c r="D101" s="170"/>
-      <c r="E101" s="153"/>
-      <c r="F101" s="186"/>
+      <c r="B101" s="208"/>
+      <c r="C101" s="209"/>
+      <c r="D101" s="213"/>
+      <c r="E101" s="209"/>
+      <c r="F101" s="216"/>
       <c r="G101" s="94" t="s">
         <v>30</v>
       </c>
@@ -10993,11 +11450,11 @@
       <c r="AP101" s="27"/>
     </row>
     <row r="102" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="152"/>
-      <c r="C102" s="153"/>
-      <c r="D102" s="170"/>
-      <c r="E102" s="153"/>
-      <c r="F102" s="186"/>
+      <c r="B102" s="208"/>
+      <c r="C102" s="209"/>
+      <c r="D102" s="213"/>
+      <c r="E102" s="209"/>
+      <c r="F102" s="216"/>
       <c r="G102" s="94" t="s">
         <v>23</v>
       </c>
@@ -11134,11 +11591,11 @@
       <c r="AP102" s="27"/>
     </row>
     <row r="103" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="152"/>
-      <c r="C103" s="153"/>
-      <c r="D103" s="170"/>
-      <c r="E103" s="153"/>
-      <c r="F103" s="186"/>
+      <c r="B103" s="208"/>
+      <c r="C103" s="209"/>
+      <c r="D103" s="213"/>
+      <c r="E103" s="209"/>
+      <c r="F103" s="216"/>
       <c r="G103" s="94" t="s">
         <v>26</v>
       </c>
@@ -11275,11 +11732,11 @@
       <c r="AP103" s="27"/>
     </row>
     <row r="104" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="152"/>
-      <c r="C104" s="153"/>
-      <c r="D104" s="170"/>
-      <c r="E104" s="153"/>
-      <c r="F104" s="186"/>
+      <c r="B104" s="208"/>
+      <c r="C104" s="209"/>
+      <c r="D104" s="213"/>
+      <c r="E104" s="209"/>
+      <c r="F104" s="216"/>
       <c r="G104" s="94" t="s">
         <v>24</v>
       </c>
@@ -11416,11 +11873,11 @@
       <c r="AP104" s="27"/>
     </row>
     <row r="105" spans="2:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="154"/>
-      <c r="C105" s="155"/>
-      <c r="D105" s="171"/>
-      <c r="E105" s="155"/>
-      <c r="F105" s="187"/>
+      <c r="B105" s="210"/>
+      <c r="C105" s="211"/>
+      <c r="D105" s="214"/>
+      <c r="E105" s="211"/>
+      <c r="F105" s="217"/>
       <c r="G105" s="99" t="s">
         <v>25</v>
       </c>
@@ -11557,13 +12014,13 @@
       <c r="AP105" s="27"/>
     </row>
     <row r="106" spans="2:43" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="134"/>
-      <c r="C106" s="135"/>
-      <c r="D106" s="140" t="s">
+      <c r="B106" s="193"/>
+      <c r="C106" s="194"/>
+      <c r="D106" s="199" t="s">
         <v>28</v>
       </c>
-      <c r="E106" s="135"/>
-      <c r="F106" s="144" t="s">
+      <c r="E106" s="194"/>
+      <c r="F106" s="203" t="s">
         <v>28</v>
       </c>
       <c r="G106" s="102" t="s">
@@ -11610,11 +12067,11 @@
       <c r="AQ106" s="34"/>
     </row>
     <row r="107" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="136"/>
-      <c r="C107" s="137"/>
-      <c r="D107" s="141"/>
-      <c r="E107" s="137"/>
-      <c r="F107" s="145"/>
+      <c r="B107" s="195"/>
+      <c r="C107" s="196"/>
+      <c r="D107" s="200"/>
+      <c r="E107" s="196"/>
+      <c r="F107" s="204"/>
       <c r="G107" s="107" t="s">
         <v>15</v>
       </c>
@@ -11659,11 +12116,11 @@
       <c r="AQ107" s="34"/>
     </row>
     <row r="108" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="136"/>
-      <c r="C108" s="137"/>
-      <c r="D108" s="141"/>
-      <c r="E108" s="137"/>
-      <c r="F108" s="145"/>
+      <c r="B108" s="195"/>
+      <c r="C108" s="196"/>
+      <c r="D108" s="200"/>
+      <c r="E108" s="196"/>
+      <c r="F108" s="204"/>
       <c r="G108" s="112" t="s">
         <v>16</v>
       </c>
@@ -11708,11 +12165,11 @@
       <c r="AQ108" s="34"/>
     </row>
     <row r="109" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="136"/>
-      <c r="C109" s="137"/>
-      <c r="D109" s="141"/>
-      <c r="E109" s="137"/>
-      <c r="F109" s="145"/>
+      <c r="B109" s="195"/>
+      <c r="C109" s="196"/>
+      <c r="D109" s="200"/>
+      <c r="E109" s="196"/>
+      <c r="F109" s="204"/>
       <c r="G109" s="112" t="s">
         <v>17</v>
       </c>
@@ -11757,11 +12214,11 @@
       <c r="AQ109" s="34"/>
     </row>
     <row r="110" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="136"/>
-      <c r="C110" s="137"/>
-      <c r="D110" s="141"/>
-      <c r="E110" s="137"/>
-      <c r="F110" s="145"/>
+      <c r="B110" s="195"/>
+      <c r="C110" s="196"/>
+      <c r="D110" s="200"/>
+      <c r="E110" s="196"/>
+      <c r="F110" s="204"/>
       <c r="G110" s="112" t="s">
         <v>18</v>
       </c>
@@ -11806,11 +12263,11 @@
       <c r="AQ110" s="34"/>
     </row>
     <row r="111" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="136"/>
-      <c r="C111" s="137"/>
-      <c r="D111" s="141"/>
-      <c r="E111" s="137"/>
-      <c r="F111" s="145"/>
+      <c r="B111" s="195"/>
+      <c r="C111" s="196"/>
+      <c r="D111" s="200"/>
+      <c r="E111" s="196"/>
+      <c r="F111" s="204"/>
       <c r="G111" s="112" t="s">
         <v>19</v>
       </c>
@@ -11855,11 +12312,11 @@
       <c r="AQ111" s="34"/>
     </row>
     <row r="112" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="136"/>
-      <c r="C112" s="137"/>
-      <c r="D112" s="141"/>
-      <c r="E112" s="137"/>
-      <c r="F112" s="145"/>
+      <c r="B112" s="195"/>
+      <c r="C112" s="196"/>
+      <c r="D112" s="200"/>
+      <c r="E112" s="196"/>
+      <c r="F112" s="204"/>
       <c r="G112" s="119" t="s">
         <v>20</v>
       </c>
@@ -11904,11 +12361,11 @@
       <c r="AQ112" s="34"/>
     </row>
     <row r="113" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="136"/>
-      <c r="C113" s="137"/>
-      <c r="D113" s="142"/>
-      <c r="E113" s="137"/>
-      <c r="F113" s="145"/>
+      <c r="B113" s="195"/>
+      <c r="C113" s="196"/>
+      <c r="D113" s="201"/>
+      <c r="E113" s="196"/>
+      <c r="F113" s="204"/>
       <c r="G113" s="112" t="s">
         <v>31</v>
       </c>
@@ -11953,11 +12410,11 @@
       <c r="AQ113" s="34"/>
     </row>
     <row r="114" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="136"/>
-      <c r="C114" s="137"/>
-      <c r="D114" s="142"/>
-      <c r="E114" s="137"/>
-      <c r="F114" s="145"/>
+      <c r="B114" s="195"/>
+      <c r="C114" s="196"/>
+      <c r="D114" s="201"/>
+      <c r="E114" s="196"/>
+      <c r="F114" s="204"/>
       <c r="G114" s="112" t="s">
         <v>23</v>
       </c>
@@ -12003,11 +12460,11 @@
       <c r="AQ114" s="34"/>
     </row>
     <row r="115" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="136"/>
-      <c r="C115" s="137"/>
-      <c r="D115" s="142"/>
-      <c r="E115" s="137"/>
-      <c r="F115" s="145"/>
+      <c r="B115" s="195"/>
+      <c r="C115" s="196"/>
+      <c r="D115" s="201"/>
+      <c r="E115" s="196"/>
+      <c r="F115" s="204"/>
       <c r="G115" s="112" t="s">
         <v>26</v>
       </c>
@@ -12052,11 +12509,11 @@
       <c r="AQ115" s="34"/>
     </row>
     <row r="116" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="136"/>
-      <c r="C116" s="137"/>
-      <c r="D116" s="142"/>
-      <c r="E116" s="137"/>
-      <c r="F116" s="145"/>
+      <c r="B116" s="195"/>
+      <c r="C116" s="196"/>
+      <c r="D116" s="201"/>
+      <c r="E116" s="196"/>
+      <c r="F116" s="204"/>
       <c r="G116" s="112" t="s">
         <v>24</v>
       </c>
@@ -12101,11 +12558,11 @@
       <c r="AQ116" s="34"/>
     </row>
     <row r="117" spans="2:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="138"/>
-      <c r="C117" s="139"/>
-      <c r="D117" s="143"/>
-      <c r="E117" s="139"/>
-      <c r="F117" s="146"/>
+      <c r="B117" s="197"/>
+      <c r="C117" s="198"/>
+      <c r="D117" s="202"/>
+      <c r="E117" s="198"/>
+      <c r="F117" s="205"/>
       <c r="G117" s="121" t="s">
         <v>25</v>
       </c>
@@ -12149,8 +12606,221 @@
       <c r="AP117" s="27"/>
       <c r="AQ117" s="34"/>
     </row>
+    <row r="118" spans="2:43" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B118" s="218" t="s">
+        <v>39</v>
+      </c>
+      <c r="C118" s="219"/>
+      <c r="D118" s="220"/>
+      <c r="E118" s="221"/>
+      <c r="F118" s="222" t="s">
+        <v>40</v>
+      </c>
+      <c r="G118" s="223">
+        <v>0</v>
+      </c>
+      <c r="H118" s="224"/>
+      <c r="I118" s="224"/>
+      <c r="J118" s="224"/>
+      <c r="K118" s="224"/>
+      <c r="L118" s="224"/>
+      <c r="M118" s="224"/>
+      <c r="N118" s="224"/>
+      <c r="O118" s="224"/>
+      <c r="P118" s="224"/>
+      <c r="Q118" s="224"/>
+      <c r="R118" s="224"/>
+      <c r="S118" s="224"/>
+      <c r="T118" s="224"/>
+      <c r="U118" s="224"/>
+      <c r="V118" s="224"/>
+      <c r="W118" s="224"/>
+      <c r="X118" s="224"/>
+      <c r="Y118" s="224"/>
+      <c r="Z118" s="224"/>
+      <c r="AA118" s="224"/>
+      <c r="AB118" s="224"/>
+      <c r="AC118" s="224"/>
+      <c r="AD118" s="224"/>
+      <c r="AE118" s="224"/>
+      <c r="AF118" s="224"/>
+      <c r="AG118" s="224"/>
+      <c r="AH118" s="224"/>
+      <c r="AI118" s="224"/>
+      <c r="AJ118" s="224"/>
+      <c r="AK118" s="224"/>
+      <c r="AL118" s="225"/>
+      <c r="AM118" s="226"/>
+      <c r="AN118" s="227">
+        <f>SUM(G118:AL118)</f>
+        <v>0</v>
+      </c>
+      <c r="AO118" s="228"/>
+    </row>
+    <row r="119" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B119" s="229" t="s">
+        <v>41</v>
+      </c>
+      <c r="C119" s="230"/>
+      <c r="D119" s="231"/>
+      <c r="E119" s="232"/>
+      <c r="F119" s="233"/>
+      <c r="G119" s="234"/>
+      <c r="H119" s="235"/>
+      <c r="I119" s="235"/>
+      <c r="J119" s="235"/>
+      <c r="K119" s="235"/>
+      <c r="L119" s="235"/>
+      <c r="M119" s="235"/>
+      <c r="N119" s="235"/>
+      <c r="O119" s="235"/>
+      <c r="P119" s="235"/>
+      <c r="Q119" s="235"/>
+      <c r="R119" s="235"/>
+      <c r="S119" s="235"/>
+      <c r="T119" s="235"/>
+      <c r="U119" s="235"/>
+      <c r="V119" s="235"/>
+      <c r="W119" s="235"/>
+      <c r="X119" s="235"/>
+      <c r="Y119" s="235"/>
+      <c r="Z119" s="235"/>
+      <c r="AA119" s="235"/>
+      <c r="AB119" s="235"/>
+      <c r="AC119" s="235"/>
+      <c r="AD119" s="235"/>
+      <c r="AE119" s="235"/>
+      <c r="AF119" s="235"/>
+      <c r="AG119" s="235"/>
+      <c r="AH119" s="235"/>
+      <c r="AI119" s="235"/>
+      <c r="AJ119" s="235"/>
+      <c r="AK119" s="235"/>
+      <c r="AL119" s="236"/>
+      <c r="AM119" s="237"/>
+      <c r="AN119" s="238">
+        <f>SUM(H119:AL119)</f>
+        <v>0</v>
+      </c>
+      <c r="AO119" s="239"/>
+    </row>
+    <row r="120" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B120" s="240" t="s">
+        <v>42</v>
+      </c>
+      <c r="C120" s="241"/>
+      <c r="D120" s="242"/>
+      <c r="E120" s="243"/>
+      <c r="F120" s="244"/>
+      <c r="G120" s="245"/>
+      <c r="H120" s="246"/>
+      <c r="I120" s="246"/>
+      <c r="J120" s="246"/>
+      <c r="K120" s="246"/>
+      <c r="L120" s="246"/>
+      <c r="M120" s="246"/>
+      <c r="N120" s="246"/>
+      <c r="O120" s="246"/>
+      <c r="P120" s="246"/>
+      <c r="Q120" s="246"/>
+      <c r="R120" s="246"/>
+      <c r="S120" s="246"/>
+      <c r="T120" s="246"/>
+      <c r="U120" s="246"/>
+      <c r="V120" s="246"/>
+      <c r="W120" s="246"/>
+      <c r="X120" s="246"/>
+      <c r="Y120" s="246"/>
+      <c r="Z120" s="246"/>
+      <c r="AA120" s="246"/>
+      <c r="AB120" s="246"/>
+      <c r="AC120" s="246"/>
+      <c r="AD120" s="246"/>
+      <c r="AE120" s="246"/>
+      <c r="AF120" s="246"/>
+      <c r="AG120" s="246"/>
+      <c r="AH120" s="246"/>
+      <c r="AI120" s="246"/>
+      <c r="AJ120" s="246"/>
+      <c r="AK120" s="246"/>
+      <c r="AL120" s="247"/>
+      <c r="AM120" s="68"/>
+      <c r="AN120" s="248">
+        <f>SUM(H120:AL120)</f>
+        <v>0</v>
+      </c>
+      <c r="AO120" s="249"/>
+    </row>
+    <row r="121" spans="2:43" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B121" s="250" t="s">
+        <v>43</v>
+      </c>
+      <c r="C121" s="251"/>
+      <c r="D121" s="252"/>
+      <c r="E121" s="253"/>
+      <c r="F121" s="254"/>
+      <c r="G121" s="255"/>
+      <c r="H121" s="256"/>
+      <c r="I121" s="256"/>
+      <c r="J121" s="256"/>
+      <c r="K121" s="256"/>
+      <c r="L121" s="256"/>
+      <c r="M121" s="256"/>
+      <c r="N121" s="256"/>
+      <c r="O121" s="256"/>
+      <c r="P121" s="256"/>
+      <c r="Q121" s="256"/>
+      <c r="R121" s="256"/>
+      <c r="S121" s="256"/>
+      <c r="T121" s="256"/>
+      <c r="U121" s="256"/>
+      <c r="V121" s="256"/>
+      <c r="W121" s="256"/>
+      <c r="X121" s="256"/>
+      <c r="Y121" s="256"/>
+      <c r="Z121" s="256"/>
+      <c r="AA121" s="256"/>
+      <c r="AB121" s="256"/>
+      <c r="AC121" s="256"/>
+      <c r="AD121" s="256"/>
+      <c r="AE121" s="256"/>
+      <c r="AF121" s="256"/>
+      <c r="AG121" s="256"/>
+      <c r="AH121" s="256"/>
+      <c r="AI121" s="256"/>
+      <c r="AJ121" s="256"/>
+      <c r="AK121" s="256"/>
+      <c r="AL121" s="257"/>
+      <c r="AM121" s="258"/>
+      <c r="AN121" s="259">
+        <f>SUM(H121:AL121)</f>
+        <v>0</v>
+      </c>
+      <c r="AO121" s="260"/>
+    </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B106:C117"/>
+    <mergeCell ref="D106:E117"/>
+    <mergeCell ref="F106:F117"/>
+    <mergeCell ref="F82:F93"/>
+    <mergeCell ref="B94:C105"/>
+    <mergeCell ref="D94:E105"/>
+    <mergeCell ref="F94:F105"/>
+    <mergeCell ref="B70:C81"/>
+    <mergeCell ref="D70:E81"/>
+    <mergeCell ref="F70:F81"/>
+    <mergeCell ref="B82:C93"/>
+    <mergeCell ref="F58:F69"/>
+    <mergeCell ref="B58:C69"/>
+    <mergeCell ref="D58:E69"/>
+    <mergeCell ref="D82:E93"/>
+    <mergeCell ref="D46:E57"/>
+    <mergeCell ref="F46:F57"/>
+    <mergeCell ref="D22:E33"/>
+    <mergeCell ref="F22:F33"/>
+    <mergeCell ref="D34:E45"/>
+    <mergeCell ref="F34:F45"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B46:C57"/>
@@ -12167,818 +12837,805 @@
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="D10:E21"/>
     <mergeCell ref="F10:F21"/>
-    <mergeCell ref="D46:E57"/>
-    <mergeCell ref="F46:F57"/>
-    <mergeCell ref="D22:E33"/>
-    <mergeCell ref="F22:F33"/>
-    <mergeCell ref="D34:E45"/>
-    <mergeCell ref="F34:F45"/>
-    <mergeCell ref="B70:C81"/>
-    <mergeCell ref="D70:E81"/>
-    <mergeCell ref="F70:F81"/>
-    <mergeCell ref="B82:C93"/>
-    <mergeCell ref="F58:F69"/>
-    <mergeCell ref="B58:C69"/>
-    <mergeCell ref="D58:E69"/>
-    <mergeCell ref="D82:E93"/>
-    <mergeCell ref="B106:C117"/>
-    <mergeCell ref="D106:E117"/>
-    <mergeCell ref="F106:F117"/>
-    <mergeCell ref="F82:F93"/>
-    <mergeCell ref="B94:C105"/>
-    <mergeCell ref="D94:E105"/>
-    <mergeCell ref="F94:F105"/>
   </mergeCells>
   <conditionalFormatting sqref="H8:AL8 AM8:AM9">
-    <cfRule type="cellIs" dxfId="197" priority="314" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="316" stopIfTrue="1" operator="equal">
       <formula>"La"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="315" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="317" stopIfTrue="1" operator="equal">
       <formula>"Su"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:AL9 H106:AL117">
-    <cfRule type="expression" dxfId="195" priority="321" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="323" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="322" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="324" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM106:AM107">
-    <cfRule type="cellIs" dxfId="193" priority="305" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="307" stopIfTrue="1" operator="equal">
       <formula>"La"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="306" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="308" stopIfTrue="1" operator="equal">
       <formula>"Su"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM35">
-    <cfRule type="cellIs" dxfId="191" priority="285" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="287" stopIfTrue="1" operator="equal">
       <formula>"La"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="286" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="288" stopIfTrue="1" operator="equal">
       <formula>"Su"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM46:AM47">
-    <cfRule type="cellIs" dxfId="189" priority="276" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="278" stopIfTrue="1" operator="equal">
       <formula>"La"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="277" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="279" stopIfTrue="1" operator="equal">
       <formula>"Su"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM58:AM59">
-    <cfRule type="cellIs" dxfId="187" priority="267" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="269" stopIfTrue="1" operator="equal">
       <formula>"La"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="268" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="270" stopIfTrue="1" operator="equal">
       <formula>"Su"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM70:AM71">
-    <cfRule type="cellIs" dxfId="185" priority="258" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="260" stopIfTrue="1" operator="equal">
       <formula>"La"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="259" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="261" stopIfTrue="1" operator="equal">
       <formula>"Su"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM82:AM83">
-    <cfRule type="cellIs" dxfId="183" priority="249" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="251" stopIfTrue="1" operator="equal">
       <formula>"La"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="250" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="252" stopIfTrue="1" operator="equal">
       <formula>"Su"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H94:AL105">
-    <cfRule type="expression" dxfId="181" priority="247" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="249" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="248" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="250" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG10:AH21 H10:AA21 AI10:AJ10">
-    <cfRule type="expression" dxfId="179" priority="245" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="247" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="246" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="248" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33:AA33 P23:P28 AG22:AG32 S23:S28 AG33:AH33">
-    <cfRule type="expression" dxfId="177" priority="243" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="245" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="244" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="246" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:AL45 H34:M44 Y35:AD44 AH35:AL44 O34:V44 Y34:AA34 AH34">
-    <cfRule type="expression" dxfId="175" priority="241" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="243" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="244" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46:AL57">
-    <cfRule type="expression" dxfId="173" priority="239" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="241" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="242" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:AL69 H58 H59:Q67 S58:X67 AA58:AL67">
-    <cfRule type="expression" dxfId="171" priority="237" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="239" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="238" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="240" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:AL81 H70:Q80 S70:X80 AA70:AL77 AA79:AL80 AA78:AE78 AG78:AL78">
-    <cfRule type="expression" dxfId="169" priority="235" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="237" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="236" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="238" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82:AL93">
-    <cfRule type="expression" dxfId="167" priority="233" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="235" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="234" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="236" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23:L29 L32">
-    <cfRule type="expression" dxfId="165" priority="221" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="223" stopIfTrue="1">
       <formula>L$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="222" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="224" stopIfTrue="1">
       <formula>L$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23:M29 M32">
-    <cfRule type="expression" dxfId="163" priority="219" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="221" stopIfTrue="1">
       <formula>M$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="220" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="222" stopIfTrue="1">
       <formula>M$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P22">
-    <cfRule type="expression" dxfId="161" priority="217" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="219" stopIfTrue="1">
       <formula>P$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="220" stopIfTrue="1">
       <formula>P$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
-    <cfRule type="expression" dxfId="159" priority="213" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="215" stopIfTrue="1">
       <formula>S$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="214" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="216" stopIfTrue="1">
       <formula>S$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P29:P32">
-    <cfRule type="expression" dxfId="157" priority="211" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="213" stopIfTrue="1">
       <formula>P$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="212" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="214" stopIfTrue="1">
       <formula>P$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S29:S32">
-    <cfRule type="expression" dxfId="155" priority="207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="209" stopIfTrue="1">
       <formula>S$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="208" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="210" stopIfTrue="1">
       <formula>S$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:Z28">
-    <cfRule type="expression" dxfId="153" priority="187" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="189" stopIfTrue="1">
       <formula>Z$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="188" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="190" stopIfTrue="1">
       <formula>Z$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z29:Z32">
-    <cfRule type="expression" dxfId="151" priority="183" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="185" stopIfTrue="1">
       <formula>Z$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="184" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="186" stopIfTrue="1">
       <formula>Z$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA23:AA28">
-    <cfRule type="expression" dxfId="149" priority="181" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="183" stopIfTrue="1">
       <formula>AA$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="182" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="184" stopIfTrue="1">
       <formula>AA$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA29:AA32">
-    <cfRule type="expression" dxfId="147" priority="177" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="179" stopIfTrue="1">
       <formula>AA$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="180" stopIfTrue="1">
       <formula>AA$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T23:T28">
-    <cfRule type="expression" dxfId="145" priority="175" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="177" stopIfTrue="1">
       <formula>T$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="178" stopIfTrue="1">
       <formula>T$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T22">
-    <cfRule type="expression" dxfId="143" priority="173" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="175" stopIfTrue="1">
       <formula>T$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="176" stopIfTrue="1">
       <formula>T$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T29:T32">
-    <cfRule type="expression" dxfId="141" priority="171" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="173" stopIfTrue="1">
       <formula>T$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="174" stopIfTrue="1">
       <formula>T$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:Q58">
-    <cfRule type="expression" dxfId="139" priority="169" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="171" stopIfTrue="1">
       <formula>I$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="172" stopIfTrue="1">
       <formula>I$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X35:X40">
-    <cfRule type="expression" dxfId="137" priority="167" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="169" stopIfTrue="1">
       <formula>X$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="168" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="170" stopIfTrue="1">
       <formula>X$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34">
-    <cfRule type="expression" dxfId="135" priority="165" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="167" stopIfTrue="1">
       <formula>X$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="166" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="168" stopIfTrue="1">
       <formula>X$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X41:X44">
-    <cfRule type="expression" dxfId="133" priority="163" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="165" stopIfTrue="1">
       <formula>X$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="164" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="166" stopIfTrue="1">
       <formula>X$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W35:W40">
-    <cfRule type="expression" dxfId="131" priority="155" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="157" stopIfTrue="1">
       <formula>W$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="158" stopIfTrue="1">
       <formula>W$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W34">
-    <cfRule type="expression" dxfId="129" priority="153" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="155" stopIfTrue="1">
       <formula>W$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="156" stopIfTrue="1">
       <formula>W$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W41:W44">
-    <cfRule type="expression" dxfId="127" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="153" stopIfTrue="1">
       <formula>W$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="154" stopIfTrue="1">
       <formula>W$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:K32 L22:O22 L30:O31">
-    <cfRule type="expression" dxfId="125" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="103" stopIfTrue="1">
       <formula>K$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="104" stopIfTrue="1">
       <formula>K$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23:N29 N32">
-    <cfRule type="expression" dxfId="123" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="101" stopIfTrue="1">
       <formula>N$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="102" stopIfTrue="1">
       <formula>N$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34:N44">
-    <cfRule type="expression" dxfId="121" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="99" stopIfTrue="1">
       <formula>N$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="100" stopIfTrue="1">
       <formula>N$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE35:AE40">
-    <cfRule type="expression" dxfId="119" priority="143" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="145" stopIfTrue="1">
       <formula>AE$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="146" stopIfTrue="1">
       <formula>AE$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q22:Q32">
-    <cfRule type="expression" dxfId="117" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="95" stopIfTrue="1">
       <formula>Q$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="96" stopIfTrue="1">
       <formula>Q$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE41:AE44">
-    <cfRule type="expression" dxfId="115" priority="139" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="141" stopIfTrue="1">
       <formula>AE$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="140" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="142" stopIfTrue="1">
       <formula>AE$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF35:AF40">
-    <cfRule type="expression" dxfId="113" priority="137" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="139" stopIfTrue="1">
       <formula>AF$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="140" stopIfTrue="1">
       <formula>AF$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22:V32">
-    <cfRule type="expression" dxfId="111" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="89" stopIfTrue="1">
       <formula>V$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="90" stopIfTrue="1">
       <formula>V$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF41:AF44">
-    <cfRule type="expression" dxfId="109" priority="133" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="135" stopIfTrue="1">
       <formula>AF$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="136" stopIfTrue="1">
       <formula>AF$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23:AH28">
-    <cfRule type="expression" dxfId="107" priority="131" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="133" stopIfTrue="1">
       <formula>AH$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="134" stopIfTrue="1">
       <formula>AH$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH22">
-    <cfRule type="expression" dxfId="105" priority="129" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="131" stopIfTrue="1">
       <formula>AH$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="132" stopIfTrue="1">
       <formula>AH$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH29:AH32">
-    <cfRule type="expression" dxfId="103" priority="127" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="129" stopIfTrue="1">
       <formula>AH$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="130" stopIfTrue="1">
       <formula>AH$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG35:AG40">
-    <cfRule type="expression" dxfId="101" priority="125" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="127" stopIfTrue="1">
       <formula>AG$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="126" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="128" stopIfTrue="1">
       <formula>AG$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG41:AG44">
-    <cfRule type="expression" dxfId="99" priority="121" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="123" stopIfTrue="1">
       <formula>AG$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="124" stopIfTrue="1">
       <formula>AG$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R59:R67">
-    <cfRule type="expression" dxfId="97" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="73" stopIfTrue="1">
       <formula>R$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="74" stopIfTrue="1">
       <formula>R$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R58">
-    <cfRule type="expression" dxfId="95" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="71" stopIfTrue="1">
       <formula>R$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="72" stopIfTrue="1">
       <formula>R$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y59:Y67">
-    <cfRule type="expression" dxfId="93" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="69" stopIfTrue="1">
       <formula>Y$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="70" stopIfTrue="1">
       <formula>Y$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U22:U32">
-    <cfRule type="expression" dxfId="91" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
       <formula>U$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="92" stopIfTrue="1">
       <formula>U$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W22:W32">
-    <cfRule type="expression" dxfId="89" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
       <formula>W$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="88" stopIfTrue="1">
       <formula>W$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H32">
-    <cfRule type="expression" dxfId="87" priority="107" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="109" stopIfTrue="1">
       <formula>H$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="110" stopIfTrue="1">
       <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:I32">
-    <cfRule type="expression" dxfId="85" priority="105" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="107" stopIfTrue="1">
       <formula>I$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="108" stopIfTrue="1">
       <formula>I$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:J32">
-    <cfRule type="expression" dxfId="83" priority="103" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="105" stopIfTrue="1">
       <formula>J$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="106" stopIfTrue="1">
       <formula>J$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23:O29 O32">
-    <cfRule type="expression" dxfId="81" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="97" stopIfTrue="1">
       <formula>O$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="98" stopIfTrue="1">
       <formula>O$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22:R32">
-    <cfRule type="expression" dxfId="79" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="93" stopIfTrue="1">
       <formula>R$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="94" stopIfTrue="1">
       <formula>R$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X23:X32">
-    <cfRule type="expression" dxfId="77" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="85" stopIfTrue="1">
       <formula>X$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="86" stopIfTrue="1">
       <formula>X$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y23:Y32">
-    <cfRule type="expression" dxfId="75" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="83" stopIfTrue="1">
       <formula>Y$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="84" stopIfTrue="1">
       <formula>Y$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X22">
-    <cfRule type="expression" dxfId="73" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="81" stopIfTrue="1">
       <formula>X$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="82" stopIfTrue="1">
       <formula>X$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y22:AC22">
-    <cfRule type="expression" dxfId="71" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="79" stopIfTrue="1">
       <formula>Y$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="80" stopIfTrue="1">
       <formula>Y$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R71:R80">
-    <cfRule type="expression" dxfId="69" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="77" stopIfTrue="1">
       <formula>R$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="78" stopIfTrue="1">
       <formula>R$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R70">
-    <cfRule type="expression" dxfId="67" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="75" stopIfTrue="1">
       <formula>R$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="76" stopIfTrue="1">
       <formula>R$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y58">
-    <cfRule type="expression" dxfId="65" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="67" stopIfTrue="1">
       <formula>Y$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="68" stopIfTrue="1">
       <formula>Y$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z59:Z67">
-    <cfRule type="expression" dxfId="63" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="65" stopIfTrue="1">
       <formula>Z$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="66" stopIfTrue="1">
       <formula>Z$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z58">
-    <cfRule type="expression" dxfId="61" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="63" stopIfTrue="1">
       <formula>Z$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="64" stopIfTrue="1">
       <formula>Z$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y80:Z80">
-    <cfRule type="expression" dxfId="59" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="61" stopIfTrue="1">
       <formula>Y$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="62" stopIfTrue="1">
       <formula>Y$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y71:Y79">
-    <cfRule type="expression" dxfId="57" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="59" stopIfTrue="1">
       <formula>Y$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="60" stopIfTrue="1">
       <formula>Y$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y70">
-    <cfRule type="expression" dxfId="55" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="57" stopIfTrue="1">
       <formula>Y$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="58" stopIfTrue="1">
       <formula>Y$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z71:Z79">
-    <cfRule type="expression" dxfId="53" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
       <formula>Z$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
       <formula>Z$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z70">
-    <cfRule type="expression" dxfId="51" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="53" stopIfTrue="1">
       <formula>Z$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="54" stopIfTrue="1">
       <formula>Z$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF78">
-    <cfRule type="expression" dxfId="49" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="51" stopIfTrue="1">
       <formula>AF$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="52" stopIfTrue="1">
       <formula>AF$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB10:AF21">
-    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="49" stopIfTrue="1">
       <formula>AB$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="50" stopIfTrue="1">
       <formula>AB$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB33:AF33">
-    <cfRule type="expression" dxfId="45" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="47" stopIfTrue="1">
       <formula>AB$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="48" stopIfTrue="1">
       <formula>AB$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB34:AC34 AF34:AG34">
-    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="45" stopIfTrue="1">
       <formula>AB$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="46" stopIfTrue="1">
       <formula>AB$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE34">
-    <cfRule type="expression" dxfId="41" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="43" stopIfTrue="1">
       <formula>AE$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="44" stopIfTrue="1">
       <formula>AE$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD34">
-    <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="41" stopIfTrue="1">
       <formula>AD$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="42" stopIfTrue="1">
       <formula>AD$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB23:AB32">
-    <cfRule type="expression" dxfId="37" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="39" stopIfTrue="1">
       <formula>AB$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="40" stopIfTrue="1">
       <formula>AB$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC23:AC32">
-    <cfRule type="expression" dxfId="35" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="37" stopIfTrue="1">
       <formula>AC$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="38" stopIfTrue="1">
       <formula>AC$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD22:AD32">
-    <cfRule type="expression" dxfId="33" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="35" stopIfTrue="1">
       <formula>AD$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="36" stopIfTrue="1">
       <formula>AD$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE23:AE32">
-    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="33" stopIfTrue="1">
       <formula>AE$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="34" stopIfTrue="1">
       <formula>AE$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF23:AF32">
-    <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="31" stopIfTrue="1">
       <formula>AF$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="32" stopIfTrue="1">
       <formula>AF$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE22">
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="29" stopIfTrue="1">
       <formula>AE$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="30" stopIfTrue="1">
       <formula>AE$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF22">
-    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="27" stopIfTrue="1">
       <formula>AF$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="28" stopIfTrue="1">
       <formula>AF$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI11:AM21 AK10:AM10">
-    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="25" stopIfTrue="1">
       <formula>AI$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="26" stopIfTrue="1">
       <formula>AI$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI33:AM33">
-    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
       <formula>AI$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
       <formula>AI$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI34:AJ34 AM34">
-    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="21" stopIfTrue="1">
       <formula>AI$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="22" stopIfTrue="1">
       <formula>AI$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL34">
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="19" stopIfTrue="1">
       <formula>AL$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="20" stopIfTrue="1">
       <formula>AL$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK34">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
       <formula>AK$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
       <formula>AK$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI22:AI32">
-    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="15" stopIfTrue="1">
       <formula>AI$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
       <formula>AI$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22:AJ32">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="13" stopIfTrue="1">
       <formula>AJ$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
       <formula>AJ$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK22:AK32">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>AK$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>AK$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL23:AL32">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
       <formula>AL$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>AL$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM23:AM32">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
       <formula>AM$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
       <formula>AM$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL22">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>AL$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>AL$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM22">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>AM$7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>AM$5=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H118:AL121">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>H$7=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+      <formula>H$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.73636363636363633" right="0.11805555555555557" top="0.35795454545454547" bottom="0.51180555555555562" header="0.51180555555555562" footer="0.51180555555555562"/>

</xml_diff>